<commit_message>
Fui ate o add address list
</commit_message>
<xml_diff>
--- a/clientesTerezinha.xlsx
+++ b/clientesTerezinha.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="154">
   <si>
     <t>aline</t>
   </si>
@@ -784,7 +784,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -792,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C234"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1508,9 +1508,1253 @@
       <c r="C78" s="1"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
+      <c r="A79" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A225" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A226" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A229" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A230" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A233" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A234" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
verificar o busca existencia
</commit_message>
<xml_diff>
--- a/clientesTerezinha.xlsx
+++ b/clientesTerezinha.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
   <si>
     <t>aline</t>
   </si>
@@ -166,9 +166,6 @@
     <t>4C:5E:0C:54:38:7B</t>
   </si>
   <si>
-    <t>4C:5E:0C:57:4B;59</t>
-  </si>
-  <si>
     <t>00:1A:3F:E0:F7:F0</t>
   </si>
   <si>
@@ -397,9 +394,6 @@
     <t>elisiane</t>
   </si>
   <si>
-    <t>elizete</t>
-  </si>
-  <si>
     <t>gisele</t>
   </si>
   <si>
@@ -442,9 +436,6 @@
     <t>marcos</t>
   </si>
   <si>
-    <t>pedro</t>
-  </si>
-  <si>
     <t>patricia</t>
   </si>
   <si>
@@ -476,6 +467,9 @@
   </si>
   <si>
     <t>08:10:74:3f:28:00</t>
+  </si>
+  <si>
+    <t>4C:5E:0C:57:4B:59</t>
   </si>
 </sst>
 </file>
@@ -784,7 +778,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -792,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C234"/>
+  <dimension ref="A1:C231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="B174" sqref="B174"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -807,7 +801,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -816,7 +810,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -834,7 +828,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -843,7 +837,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
@@ -852,7 +846,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
@@ -861,10 +855,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>121</v>
+        <v>79</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -873,7 +867,7 @@
         <v>80</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -882,7 +876,7 @@
         <v>81</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -891,16 +885,16 @@
         <v>82</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -909,7 +903,7 @@
         <v>122</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -918,16 +912,16 @@
         <v>123</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1"/>
     </row>
@@ -936,61 +930,61 @@
         <v>84</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>118</v>
+        <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="C21" s="1"/>
     </row>
@@ -999,124 +993,124 @@
         <v>87</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>88</v>
+        <v>142</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>89</v>
+        <v>126</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>90</v>
+        <v>127</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>131</v>
+        <v>90</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C30" s="1"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>133</v>
+        <v>92</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>93</v>
+        <v>133</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>135</v>
+        <v>93</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C35" s="1"/>
     </row>
@@ -1125,58 +1119,58 @@
         <v>94</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>95</v>
+        <v>132</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>134</v>
+        <v>95</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>50</v>
@@ -1221,82 +1215,82 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="C48" s="1"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="C49" s="1"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C51" s="1"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C52" s="1"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>141</v>
+        <v>9</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>59</v>
+        <v>148</v>
       </c>
       <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C54" s="1"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>151</v>
+        <v>60</v>
       </c>
       <c r="C55" s="1"/>
     </row>
@@ -1311,7 +1305,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>62</v>
@@ -1320,7 +1314,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>63</v>
@@ -1329,16 +1323,16 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>142</v>
+        <v>42</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>64</v>
@@ -1347,115 +1341,115 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C62" s="1"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C63" s="1"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="C64" s="1"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="C65" s="1"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="C66" s="1"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="C67" s="1"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C68" s="1"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C69" s="1"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>5</v>
+        <v>150</v>
       </c>
       <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="C72" s="1"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>115</v>
+        <v>146</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>73</v>
@@ -1464,19 +1458,19 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>148</v>
+        <v>115</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>153</v>
+        <v>74</v>
       </c>
       <c r="C74" s="1"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="C75" s="1"/>
     </row>
@@ -1490,1273 +1484,629 @@
       <c r="C76" s="1"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C77" s="1"/>
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C78" s="1"/>
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C79" s="1"/>
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>151</v>
-      </c>
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A134" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A138" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="A141" s="1"/>
+      <c r="B141" s="1"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="A142" s="1"/>
+      <c r="B142" s="1"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="A143" s="1"/>
+      <c r="B143" s="1"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>92</v>
-      </c>
+      <c r="A144" s="1"/>
+      <c r="B144" s="1"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>152</v>
-      </c>
+      <c r="A145" s="1"/>
+      <c r="B145" s="1"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A146" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="A147" s="1"/>
+      <c r="B147" s="1"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="A148" s="1"/>
+      <c r="B148" s="1"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A149" s="1"/>
+      <c r="B149" s="1"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="A150" s="1"/>
+      <c r="B150" s="1"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="A151" s="1"/>
+      <c r="B151" s="1"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>153</v>
-      </c>
+      <c r="A152" s="1"/>
+      <c r="B152" s="1"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="A153" s="1"/>
+      <c r="B153" s="1"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="A154" s="1"/>
+      <c r="B154" s="1"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="A155" s="1"/>
+      <c r="B155" s="1"/>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="A156" s="1"/>
+      <c r="B156" s="1"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="A157" s="1"/>
+      <c r="B157" s="1"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A158" s="1"/>
+      <c r="B158" s="1"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A159" s="1"/>
+      <c r="B159" s="1"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A160" s="1"/>
+      <c r="B160" s="1"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A161" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A161" s="1"/>
+      <c r="B161" s="1"/>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A162" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A163" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A164" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A164" s="1"/>
+      <c r="B164" s="1"/>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A165" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="A165" s="1"/>
+      <c r="B165" s="1"/>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A166" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A166" s="1"/>
+      <c r="B166" s="1"/>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A167" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="A167" s="1"/>
+      <c r="B167" s="1"/>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A168" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A168" s="1"/>
+      <c r="B168" s="1"/>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A169" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A169" s="1"/>
+      <c r="B169" s="1"/>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A170" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A171" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="A171" s="1"/>
+      <c r="B171" s="1"/>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A172" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="A172" s="1"/>
+      <c r="B172" s="1"/>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A173" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="A173" s="1"/>
+      <c r="B173" s="1"/>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A174" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="A174" s="1"/>
+      <c r="B174" s="1"/>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A175" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A176" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A176" s="1"/>
+      <c r="B176" s="1"/>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A177" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="A177" s="1"/>
+      <c r="B177" s="1"/>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A178" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="A178" s="1"/>
+      <c r="B178" s="1"/>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A179" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A179" s="1"/>
+      <c r="B179" s="1"/>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A180" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A180" s="1"/>
+      <c r="B180" s="1"/>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A181" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A181" s="1"/>
+      <c r="B181" s="1"/>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A182" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A182" s="1"/>
+      <c r="B182" s="1"/>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A183" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="A183" s="1"/>
+      <c r="B183" s="1"/>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A184" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B184" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="A184" s="1"/>
+      <c r="B184" s="1"/>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A185" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B185" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A185" s="1"/>
+      <c r="B185" s="1"/>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A186" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B186" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="A186" s="1"/>
+      <c r="B186" s="1"/>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A187" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="A187" s="1"/>
+      <c r="B187" s="1"/>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A188" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B188" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="A188" s="1"/>
+      <c r="B188" s="1"/>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A189" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B189" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A189" s="1"/>
+      <c r="B189" s="1"/>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A190" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B190" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="A190" s="1"/>
+      <c r="B190" s="1"/>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A191" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="A191" s="1"/>
+      <c r="B191" s="1"/>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A192" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B192" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="A192" s="1"/>
+      <c r="B192" s="1"/>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A193" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B193" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="A193" s="1"/>
+      <c r="B193" s="1"/>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A194" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B194" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="A194" s="1"/>
+      <c r="B194" s="1"/>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A195" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B195" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="A195" s="1"/>
+      <c r="B195" s="1"/>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A196" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B196" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="A196" s="1"/>
+      <c r="B196" s="1"/>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A197" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B197" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="A197" s="1"/>
+      <c r="B197" s="1"/>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A198" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B198" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="A198" s="1"/>
+      <c r="B198" s="1"/>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A199" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B199" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="A199" s="1"/>
+      <c r="B199" s="1"/>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A200" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="A200" s="1"/>
+      <c r="B200" s="1"/>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A201" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="A201" s="1"/>
+      <c r="B201" s="1"/>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A202" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="A202" s="1"/>
+      <c r="B202" s="1"/>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A203" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="A203" s="1"/>
+      <c r="B203" s="1"/>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A204" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A204" s="1"/>
+      <c r="B204" s="1"/>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A205" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="A205" s="1"/>
+      <c r="B205" s="1"/>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A206" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A206" s="1"/>
+      <c r="B206" s="1"/>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A207" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="A207" s="1"/>
+      <c r="B207" s="1"/>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A208" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="A208" s="1"/>
+      <c r="B208" s="1"/>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A209" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="A209" s="1"/>
+      <c r="B209" s="1"/>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A210" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B210" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="A210" s="1"/>
+      <c r="B210" s="1"/>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A211" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>151</v>
-      </c>
+      <c r="A211" s="1"/>
+      <c r="B211" s="1"/>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A212" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B212" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="A212" s="1"/>
+      <c r="B212" s="1"/>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A213" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="A213" s="1"/>
+      <c r="B213" s="1"/>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A214" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="A214" s="1"/>
+      <c r="B214" s="1"/>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A215" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A215" s="1"/>
+      <c r="B215" s="1"/>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A216" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="A216" s="1"/>
+      <c r="B216" s="1"/>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A217" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="A217" s="1"/>
+      <c r="B217" s="1"/>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A218" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B218" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="A218" s="1"/>
+      <c r="B218" s="1"/>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A219" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B219" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="A219" s="1"/>
+      <c r="B219" s="1"/>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A220" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B220" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="A220" s="1"/>
+      <c r="B220" s="1"/>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A221" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B221" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="A221" s="1"/>
+      <c r="B221" s="1"/>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A222" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B222" s="1" t="s">
-        <v>92</v>
-      </c>
+      <c r="A222" s="1"/>
+      <c r="B222" s="1"/>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A223" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B223" s="1" t="s">
-        <v>152</v>
-      </c>
+      <c r="A223" s="1"/>
+      <c r="B223" s="1"/>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A224" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B224" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A224" s="1"/>
+      <c r="B224" s="1"/>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A225" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B225" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="A225" s="1"/>
+      <c r="B225" s="1"/>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A226" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B226" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="A226" s="1"/>
+      <c r="B226" s="1"/>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A227" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B227" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A227" s="1"/>
+      <c r="B227" s="1"/>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A228" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B228" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="A228" s="1"/>
+      <c r="B228" s="1"/>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A229" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B229" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="A229" s="1"/>
+      <c r="B229" s="1"/>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A230" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B230" s="1" t="s">
-        <v>153</v>
-      </c>
+      <c r="A230" s="1"/>
+      <c r="B230" s="1"/>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A231" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B231" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A232" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B232" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A233" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B233" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A234" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B234" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="A231" s="1"/>
+      <c r="B231" s="1"/>
     </row>
   </sheetData>
+  <sortState ref="A2:B78">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>